<commit_message>
Best tuning params 1
</commit_message>
<xml_diff>
--- a/control/best_tuning_params.xlsx
+++ b/control/best_tuning_params.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,29 +436,1133 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Input</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>kP</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>kI</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>kD</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Output</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.1</v>
+        <v>320</v>
       </c>
       <c r="B2" t="n">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05555555555555555</v>
+        <v>0.01</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E2" t="n">
+        <v>69.15555555555557</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>310</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E3" t="n">
+        <v>33.03888888888888</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>300</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E4" t="n">
+        <v>33.53888888888888</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>290</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E5" t="n">
+        <v>33.98888888888889</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>280</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E6" t="n">
+        <v>34.38888888888889</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>270</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E7" t="n">
+        <v>34.73888888888889</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>260</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E8" t="n">
+        <v>35.03888888888888</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>250</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E9" t="n">
+        <v>35.28888888888888</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>240</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E10" t="n">
+        <v>35.48888888888889</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>230</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E11" t="n">
+        <v>35.63888888888889</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>220</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E12" t="n">
+        <v>35.73888888888889</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>210</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E13" t="n">
+        <v>35.78888888888888</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>200</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E14" t="n">
+        <v>35.78888888888888</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>190</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E15" t="n">
+        <v>35.73888888888889</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>180</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E16" t="n">
+        <v>35.63888888888889</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>170</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E17" t="n">
+        <v>35.48888888888889</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>160</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E18" t="n">
+        <v>35.28888888888889</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>150</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E19" t="n">
+        <v>35.03888888888889</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>140</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E20" t="n">
+        <v>34.73888888888889</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>130</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E21" t="n">
+        <v>34.38888888888889</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>120</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E22" t="n">
+        <v>33.98888888888889</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>110</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E23" t="n">
+        <v>33.53888888888889</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>100</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E24" t="n">
+        <v>33.03888888888889</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>90</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E25" t="n">
+        <v>32.48888888888889</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>80</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E26" t="n">
+        <v>31.88888888888889</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>70</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E27" t="n">
+        <v>31.23888888888889</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>60</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E28" t="n">
+        <v>30.53888888888889</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>50</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E29" t="n">
+        <v>29.78888888888889</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>40</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E30" t="n">
+        <v>28.98888888888889</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E31" t="n">
+        <v>28.13888888888889</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>20</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E32" t="n">
+        <v>27.23888888888889</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>10</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E33" t="n">
+        <v>26.28888888888889</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>0</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E34" t="n">
+        <v>25.28888888888889</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>-10</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E35" t="n">
+        <v>24.23888888888889</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E36" t="n">
+        <v>23.13888888888889</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>-30</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E37" t="n">
+        <v>21.98888888888889</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>-40</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E38" t="n">
+        <v>20.78888888888889</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>-50</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E39" t="n">
+        <v>19.53888888888889</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>-60</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E40" t="n">
+        <v>18.23888888888889</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>-70</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E41" t="n">
+        <v>16.88888888888889</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>-80</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E42" t="n">
+        <v>15.48888888888889</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E43" t="n">
+        <v>14.03888888888889</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>-100</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E44" t="n">
+        <v>12.53888888888889</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>-110</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E45" t="n">
+        <v>10.98888888888889</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>-120</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E46" t="n">
+        <v>9.388888888888889</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>-130</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E47" t="n">
+        <v>7.738888888888891</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>-140</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E48" t="n">
+        <v>6.038888888888891</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>-150</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E49" t="n">
+        <v>4.288888888888891</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>-160</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E50" t="n">
+        <v>2.48888888888889</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>-170</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.6388888888888888</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>-180</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-1.26111111111111</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>-190</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-3.211111111111113</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>-200</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-5.21111111111111</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>-210</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-7.261111111111111</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>-220</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-9.361111111111111</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>-230</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-11.51111111111111</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>-240</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-13.71111111111111</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>-250</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-15.96111111111111</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>-260</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-18.26111111111111</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>-270</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-20.61111111111111</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>-280</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-23.01111111111111</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>-290</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-25.46111111111111</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>-300</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-27.96111111111111</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>-310</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-30.51111111111111</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>-320</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-33.11111111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>